<commit_message>
working on methodology 18.04.
</commit_message>
<xml_diff>
--- a/09_Literature_Review/01_Literature Review_Blockchain_Implications for Business Models.xlsx
+++ b/09_Literature_Review/01_Literature Review_Blockchain_Implications for Business Models.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennis/Library/Mobile Documents/3L68KQB4HG~com~readdle~CommonDocuments/Documents/01_Uni/5. Semester/01_Masterarbeit/03_R_Project_MA/09_Literature_Review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5964553D-A4F6-B74B-9FD6-08F2DC964FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C298282-8A0A-AC4E-A9AB-400169EC78A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4960" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="I. Design" sheetId="31" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="436">
   <si>
     <t>2. Keywords</t>
   </si>
@@ -3165,6 +3165,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3174,6 +3186,54 @@
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3186,54 +3246,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3247,18 +3259,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3267,1313 +3267,7 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="187">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="121">
     <dxf>
       <font>
         <b val="0"/>
@@ -4650,77 +3344,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
         <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
@@ -4874,13 +3498,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color rgb="FFFFFFFF"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <right style="thin">
           <color rgb="FF000000"/>
@@ -4907,6 +3524,13 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -4944,6 +3568,566 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -5018,7 +4202,77 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
@@ -5202,7 +4456,7 @@
     <dxf>
       <border>
         <bottom style="thin">
-          <color theme="0"/>
+          <color rgb="FFFFFFFF"/>
         </bottom>
       </border>
     </dxf>
@@ -5239,6 +4493,34 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -5593,6 +4875,64 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -6179,97 +5519,97 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle511" displayName="Tabelle511" ref="B6:C9" totalsRowShown="0" headerRowDxfId="186" dataDxfId="185" tableBorderDxfId="184">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle511" displayName="Tabelle511" ref="B6:C9" totalsRowShown="0" headerRowDxfId="120" dataDxfId="119" tableBorderDxfId="118">
   <autoFilter ref="B6:C9" xr:uid="{00000000-0009-0000-0100-00000A000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Variable" dataDxfId="183"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Keywords" dataDxfId="182"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Variable" dataDxfId="117"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Keywords" dataDxfId="116"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle16" displayName="Tabelle16" ref="E6:F14" totalsRowShown="0" headerRowDxfId="181" dataDxfId="179" headerRowBorderDxfId="180" tableBorderDxfId="178">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle16" displayName="Tabelle16" ref="E6:F14" totalsRowShown="0" headerRowDxfId="115" dataDxfId="113" headerRowBorderDxfId="114" tableBorderDxfId="112">
   <autoFilter ref="E6:F14" xr:uid="{00000000-0009-0000-0100-000010000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Variable" dataDxfId="177"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Keywords" dataDxfId="176"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Variable" dataDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Keywords" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle162" displayName="Tabelle162" ref="H6:I14" totalsRowShown="0" headerRowDxfId="175" dataDxfId="173" headerRowBorderDxfId="174" tableBorderDxfId="172">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle162" displayName="Tabelle162" ref="H6:I14" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108" tableBorderDxfId="106">
   <autoFilter ref="H6:I14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Variable" dataDxfId="171"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Keywords" dataDxfId="170"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Variable" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Keywords" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabelle1943" displayName="Tabelle1943" ref="B5:J35" totalsRowShown="0" headerRowDxfId="169" dataDxfId="167" headerRowBorderDxfId="168" tableBorderDxfId="166">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabelle1943" displayName="Tabelle1943" ref="B5:J35" totalsRowShown="0" headerRowDxfId="96" dataDxfId="94" headerRowBorderDxfId="95" tableBorderDxfId="93">
   <autoFilter ref="B5:J35" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="9">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="File Name" dataDxfId="165"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Titel" dataDxfId="164"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Year" dataDxfId="163"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Relevance" dataDxfId="162"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Authors" dataDxfId="161"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Journal / Publisher" dataDxfId="160"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Ranking (SJR (2020) + Quartile)" dataDxfId="159"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="Abstract" dataDxfId="158"/>
-    <tableColumn id="8" xr3:uid="{C32195B3-AB09-2140-A11A-84EF989C081B}" name="Comment" dataDxfId="157"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="File Name" dataDxfId="92"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Titel" dataDxfId="91"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Year" dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Relevance" dataDxfId="89"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Authors" dataDxfId="88"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Journal / Publisher" dataDxfId="87"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Ranking (SJR (2020) + Quartile)" dataDxfId="86"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="Abstract" dataDxfId="85"/>
+    <tableColumn id="8" xr3:uid="{C32195B3-AB09-2140-A11A-84EF989C081B}" name="Comment" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{30CB269A-DAE9-CE49-98CE-BE5E9A9FDC3C}" name="Tabelle145124" displayName="Tabelle145124" ref="B5:J25" totalsRowShown="0" headerRowDxfId="145" dataDxfId="144" headerRowBorderDxfId="142" tableBorderDxfId="143">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{30CB269A-DAE9-CE49-98CE-BE5E9A9FDC3C}" name="Tabelle145124" displayName="Tabelle145124" ref="B5:J25" totalsRowShown="0" headerRowDxfId="79" dataDxfId="77" headerRowBorderDxfId="78" tableBorderDxfId="76">
   <autoFilter ref="B5:J25" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:H47">
     <sortCondition ref="C5:C47"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{C40321A3-A7F0-4740-89E9-49F2A14479C0}" name="File Name" dataDxfId="141"/>
-    <tableColumn id="2" xr3:uid="{913C7AF9-8D6C-3643-A6A9-0D902F735A4D}" name="Title" dataDxfId="140"/>
-    <tableColumn id="3" xr3:uid="{FC67C838-F968-394E-9056-DFDCD060DF07}" name="Year" dataDxfId="139"/>
-    <tableColumn id="4" xr3:uid="{95875AAD-3799-5F4D-8904-763BB3575D3A}" name="Relevance" dataDxfId="138"/>
-    <tableColumn id="5" xr3:uid="{EB9DBD6D-2822-5544-88B5-27FA559576C6}" name="Authors" dataDxfId="137"/>
-    <tableColumn id="6" xr3:uid="{2C017E19-B6DB-9B41-9A3C-C94F37D6DB1C}" name="Journal / Publisher" dataDxfId="136"/>
-    <tableColumn id="7" xr3:uid="{B09F784A-E0DC-0043-B8D4-D1203CA2F48B}" name="Ranking (SJR + Quartile)" dataDxfId="135"/>
-    <tableColumn id="10" xr3:uid="{A82E29DD-97DA-F44B-9642-F697DC7D0750}" name="Abstract" dataDxfId="134"/>
-    <tableColumn id="13" xr3:uid="{98662929-494F-E341-B704-1126A9A182B6}" name="Comment" dataDxfId="133"/>
+    <tableColumn id="1" xr3:uid="{C40321A3-A7F0-4740-89E9-49F2A14479C0}" name="File Name" dataDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{913C7AF9-8D6C-3643-A6A9-0D902F735A4D}" name="Title" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{FC67C838-F968-394E-9056-DFDCD060DF07}" name="Year" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{95875AAD-3799-5F4D-8904-763BB3575D3A}" name="Relevance" dataDxfId="72"/>
+    <tableColumn id="5" xr3:uid="{EB9DBD6D-2822-5544-88B5-27FA559576C6}" name="Authors" dataDxfId="71"/>
+    <tableColumn id="6" xr3:uid="{2C017E19-B6DB-9B41-9A3C-C94F37D6DB1C}" name="Journal / Publisher" dataDxfId="70"/>
+    <tableColumn id="7" xr3:uid="{B09F784A-E0DC-0043-B8D4-D1203CA2F48B}" name="Ranking (SJR + Quartile)" dataDxfId="69"/>
+    <tableColumn id="10" xr3:uid="{A82E29DD-97DA-F44B-9642-F697DC7D0750}" name="Abstract" dataDxfId="68"/>
+    <tableColumn id="13" xr3:uid="{98662929-494F-E341-B704-1126A9A182B6}" name="Comment" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabelle14512" displayName="Tabelle14512" ref="B5:H16" totalsRowShown="0" headerRowDxfId="156" dataDxfId="154" headerRowBorderDxfId="155" tableBorderDxfId="153">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabelle14512" displayName="Tabelle14512" ref="B5:H16" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
   <autoFilter ref="B5:H16" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:F37">
     <sortCondition ref="C5:C37"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="File Name" dataDxfId="152"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Title" dataDxfId="151"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Year" dataDxfId="150"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Relevance" dataDxfId="149"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Publisher" dataDxfId="148"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Abstract / Summary" dataDxfId="147"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="Comment" dataDxfId="146"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="File Name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Title" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Year" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Relevance" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Publisher" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Abstract / Summary" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="Comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6578,7 +5918,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6595,11 +5935,11 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="23" x14ac:dyDescent="0.25">
-      <c r="B2" s="226" t="s">
+      <c r="B2" s="230" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="226"/>
-      <c r="D2" s="226"/>
+      <c r="C2" s="230"/>
+      <c r="D2" s="230"/>
     </row>
     <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B4" s="21"/>
@@ -6614,10 +5954,10 @@
       <c r="D5" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="227" t="s">
+      <c r="E5" s="231" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="228"/>
+      <c r="F5" s="232"/>
     </row>
     <row r="6" spans="1:6" ht="31.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="76" t="s">
@@ -6771,20 +6111,20 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
-      <c r="B5" s="242" t="s">
+      <c r="B5" s="233" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="242"/>
+      <c r="C5" s="233"/>
       <c r="D5" s="17"/>
-      <c r="E5" s="242" t="s">
+      <c r="E5" s="233" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="242"/>
+      <c r="F5" s="233"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="242" t="s">
+      <c r="H5" s="233" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="242"/>
+      <c r="I5" s="233"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="33"/>
@@ -6964,24 +6304,24 @@
     </row>
     <row r="16" spans="1:10" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="16"/>
-      <c r="C16" s="246" t="s">
+      <c r="C16" s="237" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="247"/>
-      <c r="E16" s="247"/>
-      <c r="F16" s="247"/>
-      <c r="G16" s="248"/>
+      <c r="D16" s="238"/>
+      <c r="E16" s="238"/>
+      <c r="F16" s="238"/>
+      <c r="G16" s="239"/>
       <c r="H16" s="98"/>
     </row>
     <row r="17" spans="1:12" s="22" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="16"/>
-      <c r="C17" s="243" t="s">
+      <c r="C17" s="234" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="244"/>
-      <c r="E17" s="244"/>
-      <c r="F17" s="244"/>
-      <c r="G17" s="245"/>
+      <c r="D17" s="235"/>
+      <c r="E17" s="235"/>
+      <c r="F17" s="235"/>
+      <c r="G17" s="236"/>
       <c r="H17" s="49"/>
       <c r="I17" s="19"/>
     </row>
@@ -6995,65 +6335,65 @@
     </row>
     <row r="19" spans="1:12" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="33"/>
-      <c r="B19" s="234" t="s">
+      <c r="B19" s="240" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="234"/>
-      <c r="D19" s="234"/>
-      <c r="E19" s="234"/>
-      <c r="F19" s="234"/>
-      <c r="G19" s="234"/>
-      <c r="H19" s="234"/>
-      <c r="I19" s="234"/>
+      <c r="C19" s="240"/>
+      <c r="D19" s="240"/>
+      <c r="E19" s="240"/>
+      <c r="F19" s="240"/>
+      <c r="G19" s="240"/>
+      <c r="H19" s="240"/>
+      <c r="I19" s="240"/>
     </row>
     <row r="20" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="16"/>
-      <c r="B20" s="233" t="s">
+      <c r="B20" s="248" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="233"/>
-      <c r="D20" s="233" t="s">
+      <c r="C20" s="248"/>
+      <c r="D20" s="248" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="233"/>
-      <c r="F20" s="233" t="s">
+      <c r="E20" s="248"/>
+      <c r="F20" s="248" t="s">
         <v>86</v>
       </c>
-      <c r="G20" s="233"/>
-      <c r="H20" s="233"/>
-      <c r="I20" s="233"/>
+      <c r="G20" s="248"/>
+      <c r="H20" s="248"/>
+      <c r="I20" s="248"/>
     </row>
     <row r="21" spans="1:12" s="14" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="33"/>
-      <c r="B21" s="241" t="s">
+      <c r="B21" s="247" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="240"/>
-      <c r="D21" s="235" t="s">
+      <c r="C21" s="246"/>
+      <c r="D21" s="241" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="236"/>
-      <c r="F21" s="231" t="s">
+      <c r="E21" s="242"/>
+      <c r="F21" s="251" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="232"/>
-      <c r="H21" s="232"/>
-      <c r="I21" s="232"/>
+      <c r="G21" s="252"/>
+      <c r="H21" s="252"/>
+      <c r="I21" s="252"/>
     </row>
     <row r="22" spans="1:12" s="22" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="33"/>
-      <c r="B22" s="239" t="s">
+      <c r="B22" s="245" t="s">
         <v>89</v>
       </c>
-      <c r="C22" s="240"/>
-      <c r="D22" s="237" t="s">
+      <c r="C22" s="246"/>
+      <c r="D22" s="243" t="s">
         <v>90</v>
       </c>
-      <c r="E22" s="238"/>
-      <c r="F22" s="232"/>
-      <c r="G22" s="232"/>
-      <c r="H22" s="232"/>
-      <c r="I22" s="232"/>
+      <c r="E22" s="244"/>
+      <c r="F22" s="252"/>
+      <c r="G22" s="252"/>
+      <c r="H22" s="252"/>
+      <c r="I22" s="252"/>
     </row>
     <row r="23" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="33"/>
@@ -7065,29 +6405,29 @@
     </row>
     <row r="25" spans="1:12" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="33"/>
-      <c r="B25" s="229" t="s">
+      <c r="B25" s="249" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="229"/>
-      <c r="D25" s="229"/>
-      <c r="E25" s="229"/>
-      <c r="F25" s="229"/>
-      <c r="G25" s="229"/>
-      <c r="H25" s="229"/>
-      <c r="I25" s="229"/>
+      <c r="C25" s="249"/>
+      <c r="D25" s="249"/>
+      <c r="E25" s="249"/>
+      <c r="F25" s="249"/>
+      <c r="G25" s="249"/>
+      <c r="H25" s="249"/>
+      <c r="I25" s="249"/>
     </row>
     <row r="26" spans="1:12" s="12" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="33"/>
-      <c r="B26" s="230" t="s">
+      <c r="B26" s="250" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="230"/>
-      <c r="D26" s="230"/>
-      <c r="E26" s="230"/>
-      <c r="F26" s="230"/>
-      <c r="G26" s="230"/>
-      <c r="H26" s="230"/>
-      <c r="I26" s="230"/>
+      <c r="C26" s="250"/>
+      <c r="D26" s="250"/>
+      <c r="E26" s="250"/>
+      <c r="F26" s="250"/>
+      <c r="G26" s="250"/>
+      <c r="H26" s="250"/>
+      <c r="I26" s="250"/>
     </row>
     <row r="27" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="33"/>
@@ -7186,22 +6526,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="F21:I22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:I20"/>
     <mergeCell ref="B19:I19"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B25:I25"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="F21:I22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C16:G16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D21" r:id="rId1" xr:uid="{A8760928-B3A3-A942-B7AB-EB5DDC395344}"/>
@@ -7386,10 +6726,10 @@
   <dimension ref="A1:M175"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="77" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8814,27 +8154,27 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="H6:H35">
-    <cfRule type="containsText" dxfId="100" priority="4" operator="containsText" text="no ranking">
+    <cfRule type="containsText" dxfId="103" priority="4" operator="containsText" text="no ranking">
       <formula>NOT(ISERROR(SEARCH("no ranking",H6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="5" operator="containsText" text="Q3">
+    <cfRule type="containsText" dxfId="102" priority="5" operator="containsText" text="Q3">
       <formula>NOT(ISERROR(SEARCH("Q3",H6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="6" operator="containsText" text="Q2">
+    <cfRule type="containsText" dxfId="101" priority="6" operator="containsText" text="Q2">
       <formula>NOT(ISERROR(SEARCH("Q2",H6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="7" operator="containsText" text="Q1">
+    <cfRule type="containsText" dxfId="100" priority="7" operator="containsText" text="Q1">
       <formula>NOT(ISERROR(SEARCH("Q1",H6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C35">
-    <cfRule type="duplicateValues" dxfId="96" priority="283"/>
+    <cfRule type="duplicateValues" dxfId="99" priority="283"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C35">
-    <cfRule type="duplicateValues" dxfId="95" priority="286"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="286"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B35">
-    <cfRule type="duplicateValues" dxfId="94" priority="287"/>
+    <cfRule type="duplicateValues" dxfId="97" priority="287"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="2" orientation="portrait" r:id="rId1"/>
@@ -8852,11 +8192,11 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C2" sqref="C2"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9626,16 +8966,16 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="H6:H35">
-    <cfRule type="containsText" dxfId="93" priority="1" operator="containsText" text="not">
+    <cfRule type="containsText" dxfId="83" priority="1" operator="containsText" text="not">
       <formula>NOT(ISERROR(SEARCH("not",H6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="2" operator="containsText" text="Q3">
+    <cfRule type="containsText" dxfId="82" priority="2" operator="containsText" text="Q3">
       <formula>NOT(ISERROR(SEARCH("Q3",H6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="3" operator="containsText" text="Q2">
+    <cfRule type="containsText" dxfId="81" priority="3" operator="containsText" text="Q2">
       <formula>NOT(ISERROR(SEARCH("Q2",H6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="4" operator="containsText" text="Q1">
+    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="Q1">
       <formula>NOT(ISERROR(SEARCH("Q1",H6)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9658,7 +8998,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G43" sqref="G43"/>
+      <selection pane="bottomRight" activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9686,22 +9026,22 @@
       <c r="I3" s="19"/>
     </row>
     <row r="4" spans="2:10" ht="29.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="250" t="s">
+      <c r="B4" s="254" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="249" t="s">
+      <c r="C4" s="253" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="249"/>
-      <c r="E4" s="249"/>
-      <c r="F4" s="249"/>
-      <c r="G4" s="249"/>
-      <c r="H4" s="249"/>
-      <c r="I4" s="249"/>
+      <c r="D4" s="253"/>
+      <c r="E4" s="253"/>
+      <c r="F4" s="253"/>
+      <c r="G4" s="253"/>
+      <c r="H4" s="253"/>
+      <c r="I4" s="253"/>
       <c r="J4" s="19"/>
     </row>
     <row r="5" spans="2:10" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="250"/>
+      <c r="B5" s="254"/>
       <c r="C5" s="166" t="s">
         <v>97</v>
       </c>
@@ -9743,9 +9083,7 @@
       <c r="C7" s="169" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="169" t="s">
-        <v>134</v>
-      </c>
+      <c r="D7" s="169"/>
       <c r="E7" s="169"/>
       <c r="F7" s="169" t="s">
         <v>134</v>
@@ -10541,34 +9879,34 @@
       <c r="I53" s="168"/>
     </row>
     <row r="54" spans="2:9" s="198" customFormat="1" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="256" t="s">
+      <c r="B54" s="228" t="s">
         <v>434</v>
       </c>
-      <c r="C54" s="257">
+      <c r="C54" s="229">
         <f>COUNTIF(C6:C53,"x")</f>
         <v>41</v>
       </c>
-      <c r="D54" s="257">
+      <c r="D54" s="229">
         <f t="shared" ref="D54:I54" si="0">COUNTIF(D6:D53,"x")</f>
-        <v>10</v>
-      </c>
-      <c r="E54" s="257">
+        <v>9</v>
+      </c>
+      <c r="E54" s="229">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="F54" s="257">
+      <c r="F54" s="229">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G54" s="257">
+      <c r="G54" s="229">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="H54" s="257">
+      <c r="H54" s="229">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I54" s="257">
+      <c r="I54" s="229">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -10580,82 +9918,82 @@
   </mergeCells>
   <phoneticPr fontId="33" type="noConversion"/>
   <conditionalFormatting sqref="B6:B7">
-    <cfRule type="duplicateValues" dxfId="59" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="58" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="57" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="56" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="55" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="54" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="53" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="52" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="51" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="50" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="49" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="48" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="47" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="46" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="45" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="44" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="43" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="42" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="duplicateValues" dxfId="41" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="duplicateValues" dxfId="40" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="39" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="duplicateValues" dxfId="38" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="duplicateValues" dxfId="37" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:B32">
-    <cfRule type="duplicateValues" dxfId="36" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="duplicateValues" dxfId="35" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:B37">
-    <cfRule type="duplicateValues" dxfId="34" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10670,10 +10008,10 @@
   <dimension ref="B2:AD54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H58" sqref="H58"/>
+      <selection pane="bottomRight" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10752,33 +10090,33 @@
       <c r="AD3" s="41"/>
     </row>
     <row r="4" spans="2:30" ht="40.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="251" t="s">
+      <c r="B4" s="255" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="252" t="s">
+      <c r="C4" s="256" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="252"/>
-      <c r="E4" s="252"/>
-      <c r="F4" s="252"/>
-      <c r="G4" s="252"/>
-      <c r="H4" s="252"/>
-      <c r="I4" s="252"/>
-      <c r="J4" s="252"/>
-      <c r="K4" s="252"/>
-      <c r="L4" s="252"/>
-      <c r="M4" s="252"/>
-      <c r="N4" s="252"/>
-      <c r="O4" s="252"/>
+      <c r="D4" s="256"/>
+      <c r="E4" s="256"/>
+      <c r="F4" s="256"/>
+      <c r="G4" s="256"/>
+      <c r="H4" s="256"/>
+      <c r="I4" s="256"/>
+      <c r="J4" s="256"/>
+      <c r="K4" s="256"/>
+      <c r="L4" s="256"/>
+      <c r="M4" s="256"/>
+      <c r="N4" s="256"/>
+      <c r="O4" s="256"/>
       <c r="P4" s="141"/>
       <c r="Q4" s="141"/>
-      <c r="R4" s="253"/>
-      <c r="S4" s="253"/>
+      <c r="R4" s="257"/>
+      <c r="S4" s="257"/>
       <c r="T4" s="48"/>
       <c r="U4" s="48"/>
       <c r="V4" s="48"/>
-      <c r="W4" s="253"/>
-      <c r="X4" s="253"/>
+      <c r="W4" s="257"/>
+      <c r="X4" s="257"/>
       <c r="Y4" s="48"/>
       <c r="Z4" s="13"/>
       <c r="AA4" s="13"/>
@@ -10787,14 +10125,14 @@
       <c r="AD4" s="41"/>
     </row>
     <row r="5" spans="2:30" ht="114" x14ac:dyDescent="0.15">
-      <c r="B5" s="251"/>
+      <c r="B5" s="255"/>
       <c r="C5" s="164" t="s">
         <v>312</v>
       </c>
       <c r="D5" s="165" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="254" t="s">
+      <c r="E5" s="226" t="s">
         <v>110</v>
       </c>
       <c r="F5" s="165" t="s">
@@ -11919,58 +11257,58 @@
       <c r="O53" s="168"/>
     </row>
     <row r="54" spans="2:15" s="198" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="256" t="s">
+      <c r="B54" s="228" t="s">
         <v>434</v>
       </c>
-      <c r="C54" s="257">
+      <c r="C54" s="229">
         <f>COUNTIF(C6:C53,"x")</f>
         <v>18</v>
       </c>
-      <c r="D54" s="257">
+      <c r="D54" s="229">
         <f t="shared" ref="D54:N54" si="0">COUNTIF(D6:D53,"x")</f>
         <v>5</v>
       </c>
-      <c r="E54" s="257">
+      <c r="E54" s="229">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F54" s="257">
+      <c r="F54" s="229">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G54" s="257">
+      <c r="G54" s="229">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="H54" s="257">
+      <c r="H54" s="229">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="I54" s="257">
+      <c r="I54" s="229">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J54" s="257">
+      <c r="J54" s="229">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K54" s="257">
+      <c r="K54" s="229">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="L54" s="257">
+      <c r="L54" s="229">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M54" s="257">
+      <c r="M54" s="229">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N54" s="257">
+      <c r="N54" s="229">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="O54" s="257">
+      <c r="O54" s="229">
         <f>COUNTIF(O6:O53,"x")</f>
         <v>2</v>
       </c>
@@ -11984,94 +11322,94 @@
   </mergeCells>
   <phoneticPr fontId="33" type="noConversion"/>
   <conditionalFormatting sqref="B6:B7">
-    <cfRule type="duplicateValues" dxfId="89" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="88" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="87" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="86" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="85" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="84" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="83" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="82" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="81" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="80" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="79" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="78" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="77" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="76" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="75" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="74" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="73" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="72" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="duplicateValues" dxfId="71" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="duplicateValues" dxfId="70" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="69" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="duplicateValues" dxfId="68" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="duplicateValues" dxfId="67" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:B31">
-    <cfRule type="duplicateValues" dxfId="66" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="duplicateValues" dxfId="65" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33:B37">
-    <cfRule type="duplicateValues" dxfId="64" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38:B48 B50">
-    <cfRule type="duplicateValues" dxfId="63" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
-    <cfRule type="duplicateValues" dxfId="62" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="duplicateValues" dxfId="61" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:B53">
-    <cfRule type="duplicateValues" dxfId="60" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12391,7 +11729,7 @@
       <c r="B16" s="221" t="s">
         <v>430</v>
       </c>
-      <c r="C16" s="255" t="s">
+      <c r="C16" s="227" t="s">
         <v>432</v>
       </c>
       <c r="D16" s="203">

</xml_diff>